<commit_message>
BEC Tabulation Tables updated.
</commit_message>
<xml_diff>
--- a/data/open/bec_classification.xlsx
+++ b/data/open/bec_classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\business_enterprise_census_2022\data\open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C2DB7F-48CF-4AA8-A362-68D40383F5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C05DD2F-74F3-4EEF-87D4-ABF302F1FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="947" firstSheet="39" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enumerators" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="position" sheetId="4" r:id="rId4"/>
     <sheet name="owner_sex" sheetId="5" r:id="rId5"/>
     <sheet name="owner_character" sheetId="6" r:id="rId6"/>
-    <sheet name="employee_character" sheetId="7" r:id="rId7"/>
-    <sheet name="employee_sex" sheetId="8" r:id="rId8"/>
-    <sheet name="registered" sheetId="9" r:id="rId9"/>
+    <sheet name="registered" sheetId="9" r:id="rId7"/>
+    <sheet name="employee_character" sheetId="7" r:id="rId8"/>
+    <sheet name="employee_sex" sheetId="8" r:id="rId9"/>
     <sheet name="ynRegistered" sheetId="10" r:id="rId10"/>
     <sheet name="other_unitsprovince" sheetId="11" r:id="rId11"/>
     <sheet name="other_unitsisland" sheetId="12" r:id="rId12"/>
@@ -663,7 +663,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="1221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="1243">
   <si>
     <t>province</t>
   </si>
@@ -4326,6 +4326,72 @@
   </si>
   <si>
     <t>intBus8</t>
+  </si>
+  <si>
+    <t>becPilotCawi1</t>
+  </si>
+  <si>
+    <t>becPilotCawi2</t>
+  </si>
+  <si>
+    <t>becPilotCawi3</t>
+  </si>
+  <si>
+    <t>becPilotCawi4</t>
+  </si>
+  <si>
+    <t>becPilotCawi5</t>
+  </si>
+  <si>
+    <t>becPilotCawi6</t>
+  </si>
+  <si>
+    <t>becPilotCawi7</t>
+  </si>
+  <si>
+    <t>becPilotCawi8</t>
+  </si>
+  <si>
+    <t>becPilotCawi9</t>
+  </si>
+  <si>
+    <t>Chinese Cake Shop</t>
+  </si>
+  <si>
+    <t>Jessy Kweiviravaka Vatoko</t>
+  </si>
+  <si>
+    <t>Juliette Gersom</t>
+  </si>
+  <si>
+    <t>Teddy Sam Garae</t>
+  </si>
+  <si>
+    <t>Morgan's Driving school</t>
+  </si>
+  <si>
+    <t>Smol Vilij Production</t>
+  </si>
+  <si>
+    <t>Freedah Rachel Kalo</t>
+  </si>
+  <si>
+    <t>David Tamata &amp; Lineth Tamata</t>
+  </si>
+  <si>
+    <t>Coconut Palms Resort</t>
+  </si>
+  <si>
+    <t>hqBus1</t>
+  </si>
+  <si>
+    <t>hqBus2</t>
+  </si>
+  <si>
+    <t>Meroline</t>
+  </si>
+  <si>
+    <t>Domayne</t>
   </si>
 </sst>
 </file>
@@ -5234,15 +5300,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -5315,6 +5382,94 @@
       </c>
       <c r="B9" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1242</v>
       </c>
     </row>
   </sheetData>
@@ -6826,7 +6981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7581,7 +7736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -8137,7 +8292,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8694,8 +8849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8908,7 +9063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9639,8 +9794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:B239"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11570,8 +11725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:B420"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14949,7 +15104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:B551"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A531" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -19841,7 +19996,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20121,7 +20276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -20336,8 +20491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21072,6 +21227,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -21106,7 +21264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:B239"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A219" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -23037,7 +23195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:B420"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A400" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -26416,7 +26574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:B551"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A531" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -30964,8 +31122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31793,6 +31951,48 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -31843,7 +32043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -31880,46 +32080,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>